<commit_message>
Created CRDC section test scripts
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C183002-4745-46FB-9FEC-546F3D048CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22BCC2F-4AAB-462D-B05B-4B2EB18A918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sec-codes" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,13 @@
     <t>sec-backup-codes</t>
   </si>
   <si>
-    <t>MBW9S0Z709ZQ</t>
+    <t>AFTNPNN8Q880</t>
   </si>
   <si>
-    <t>K9P25VKWMY15</t>
+    <t>Z60XTEFFEGXY</t>
   </si>
   <si>
-    <t>7Z05T96S4BRR</t>
+    <t>XM4AM2PNJY0C</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Created Crdc TC02 and Crdc class
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22BCC2F-4AAB-462D-B05B-4B2EB18A918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FABF1BE-1904-4668-BD2E-0685CB961565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="648" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sec-codes" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>sec-backup-codes</t>
   </si>
   <si>
-    <t>AFTNPNN8Q880</t>
-  </si>
-  <si>
-    <t>Z60XTEFFEGXY</t>
-  </si>
-  <si>
-    <t>XM4AM2PNJY0C</t>
+    <t>SZ5TCJ42NKEA</t>
+  </si>
+  <si>
+    <t>BYH6BYARV86T</t>
+  </si>
+  <si>
+    <t>YK1J90E88BG6</t>
+  </si>
+  <si>
+    <t>CWNRQHM7CMQ3</t>
+  </si>
+  <si>
+    <t>PQYKR4S0SCAE</t>
+  </si>
+  <si>
+    <t>HB2TNX3R72X2</t>
+  </si>
+  <si>
+    <t>NP11MCW57D3V</t>
   </si>
 </sst>
 </file>
@@ -354,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,6 +397,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new login backup codes
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\CRDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FABF1BE-1904-4668-BD2E-0685CB961565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21A99C0-05FE-49C3-8A24-B434093DC562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="648" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sec-codes" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sec-backup-codes</t>
   </si>
   <si>
-    <t>SZ5TCJ42NKEA</t>
-  </si>
-  <si>
-    <t>BYH6BYARV86T</t>
-  </si>
-  <si>
-    <t>YK1J90E88BG6</t>
-  </si>
-  <si>
-    <t>CWNRQHM7CMQ3</t>
-  </si>
-  <si>
-    <t>PQYKR4S0SCAE</t>
-  </si>
-  <si>
-    <t>HB2TNX3R72X2</t>
-  </si>
-  <si>
-    <t>NP11MCW57D3V</t>
+    <t>1CZV4VTHGTVN</t>
+  </si>
+  <si>
+    <t>51K0DF5KCN34</t>
+  </si>
+  <si>
+    <t>HQT8HMXSF63S</t>
+  </si>
+  <si>
+    <t>5A41AVCX9PFR</t>
+  </si>
+  <si>
+    <t>1YA1484DG5R7</t>
+  </si>
+  <si>
+    <t>MJ6J3N01MN75</t>
+  </si>
+  <si>
+    <t>B9AV6NE42R8W</t>
+  </si>
+  <si>
+    <t>V2A2ZKV148W8</t>
+  </si>
+  <si>
+    <t>DY9R3Z05BNS8</t>
   </si>
 </sst>
 </file>
@@ -64,12 +70,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,7 +391,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -397,24 +410,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added wait to pi function
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A3F76-CAA4-4351-9249-F76780EE3094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C41EEC5-9612-4090-B18E-4718339FB818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>sec-backup-codes</t>
-  </si>
-  <si>
-    <t>51K0DF5KCN34</t>
-  </si>
-  <si>
-    <t>HQT8HMXSF63S</t>
-  </si>
-  <si>
-    <t>5A41AVCX9PFR</t>
   </si>
   <si>
     <t>1YA1484DG5R7</t>
@@ -379,7 +370,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,29 +398,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added backup codes for crdc
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C41EEC5-9612-4090-B18E-4718339FB818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9CC1B-F327-40DB-9B37-A2AAA7A34E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>sec-backup-codes</t>
-  </si>
-  <si>
-    <t>1YA1484DG5R7</t>
-  </si>
-  <si>
-    <t>MJ6J3N01MN75</t>
-  </si>
-  <si>
-    <t>B9AV6NE42R8W</t>
   </si>
   <si>
     <t>V2A2ZKV148W8</t>
@@ -370,7 +361,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,24 +379,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Crdc login backup codes
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B9CC1B-F327-40DB-9B37-A2AAA7A34E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9754ACCB-6CF7-4F59-8B05-D76EB1049CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>sec-backup-codes</t>
   </si>
   <si>
-    <t>V2A2ZKV148W8</t>
-  </si>
-  <si>
-    <t>DY9R3Z05BNS8</t>
+    <t>B5M3N2BW0MA3</t>
+  </si>
+  <si>
+    <t>XA43JHAGQ8V3</t>
+  </si>
+  <si>
+    <t>TK50GFCXFHCN</t>
+  </si>
+  <si>
+    <t>9M1A883VTX21</t>
+  </si>
+  <si>
+    <t>D2ANGGG71FGC</t>
+  </si>
+  <si>
+    <t>8AW7QA18SBTA</t>
+  </si>
+  <si>
+    <t>EA5XZ049QR7S</t>
+  </si>
+  <si>
+    <t>PTV3TSFPBF6W</t>
+  </si>
+  <si>
+    <t>NHYK5008HQDA</t>
+  </si>
+  <si>
+    <t>ZADGNDVPP03M</t>
   </si>
 </sst>
 </file>
@@ -358,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,9 +403,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added crdc backup codes
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9754ACCB-6CF7-4F59-8B05-D76EB1049CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67ED180-F085-47D2-ADF3-99E613E65832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>sec-backup-codes</t>
-  </si>
-  <si>
-    <t>B5M3N2BW0MA3</t>
-  </si>
-  <si>
-    <t>XA43JHAGQ8V3</t>
   </si>
   <si>
     <t>TK50GFCXFHCN</t>
@@ -385,7 +379,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,39 +407,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added crdc login backup code
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01968FA2-66D1-421E-9001-291DCB94B6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7C5799-4ABC-4192-90D0-253755FAE872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>sec-backup-codes</t>
-  </si>
-  <si>
-    <t>8AW7QA18SBTA</t>
-  </si>
-  <si>
-    <t>EA5XZ049QR7S</t>
-  </si>
-  <si>
-    <t>PTV3TSFPBF6W</t>
   </si>
   <si>
     <t>NHYK5008HQDA</t>
@@ -370,7 +361,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,24 +379,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created crdc calendar function
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701675B7-A67F-40FA-B5C6-FC64A414FA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9522BC88-C074-409F-84A7-2812583F8AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26203" yWindow="-609" windowWidth="17280" windowHeight="8966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26777" yWindow="2306" windowWidth="17280" windowHeight="8965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sec-codes" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sec-backup-codes</t>
   </si>
   <si>
-    <t>7VADX0RWN3NT</t>
-  </si>
-  <si>
-    <t>AA4GDR1CGGRM</t>
-  </si>
-  <si>
-    <t>VB8SVSWCP89Z</t>
-  </si>
-  <si>
-    <t>20P7SKTWSCG7</t>
-  </si>
-  <si>
-    <t>2578DVHZ2NY8</t>
-  </si>
-  <si>
-    <t>05TDN56XHKZ0</t>
-  </si>
-  <si>
-    <t>3WKDV7ZXQN1Y</t>
+    <t>QS3W554CY3ZX</t>
+  </si>
+  <si>
+    <t>Q8YK0WWBPD6H</t>
+  </si>
+  <si>
+    <t>YYZGQ1P8K4EG</t>
+  </si>
+  <si>
+    <t>3Z6ADAYX8TXX</t>
+  </si>
+  <si>
+    <t>96R6XXZ5H6HD</t>
+  </si>
+  <si>
+    <t>51XZBTACEQGM</t>
+  </si>
+  <si>
+    <t>T91KP1V5CTSN</t>
+  </si>
+  <si>
+    <t>YW0AXXBBWGJP</t>
+  </si>
+  <si>
+    <t>KBN7HS57G4H3</t>
   </si>
 </sst>
 </file>
@@ -373,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,24 +410,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Crdc element issue
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9522BC88-C074-409F-84A7-2812583F8AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB5EDC1-62F7-4C9A-8622-A7B94F0840C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26777" yWindow="2306" windowWidth="17280" windowHeight="8965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sec-codes" sheetId="1" r:id="rId1"/>
@@ -30,31 +30,31 @@
     <t>sec-backup-codes</t>
   </si>
   <si>
-    <t>QS3W554CY3ZX</t>
-  </si>
-  <si>
-    <t>Q8YK0WWBPD6H</t>
-  </si>
-  <si>
-    <t>YYZGQ1P8K4EG</t>
-  </si>
-  <si>
-    <t>3Z6ADAYX8TXX</t>
-  </si>
-  <si>
-    <t>96R6XXZ5H6HD</t>
-  </si>
-  <si>
-    <t>51XZBTACEQGM</t>
-  </si>
-  <si>
-    <t>T91KP1V5CTSN</t>
-  </si>
-  <si>
-    <t>YW0AXXBBWGJP</t>
-  </si>
-  <si>
-    <t>KBN7HS57G4H3</t>
+    <t>HKDJB5BA6J6M</t>
+  </si>
+  <si>
+    <t>04F5PQ59MWV6</t>
+  </si>
+  <si>
+    <t>95SY88G93C56</t>
+  </si>
+  <si>
+    <t>C9DEXVFAR31A</t>
+  </si>
+  <si>
+    <t>05ANDJ337D9B</t>
+  </si>
+  <si>
+    <t>SAS5DZQK4GHR</t>
+  </si>
+  <si>
+    <t>YC7CEVJY9735</t>
+  </si>
+  <si>
+    <t>X36KP2Z510RZ</t>
+  </si>
+  <si>
+    <t>MK83F9RSV97N</t>
   </si>
 </sst>
 </file>
@@ -379,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,46 +397,46 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added CCDI 5 scripts and C3DC structure
</commit_message>
<xml_diff>
--- a/InputFiles/CRDC/BackupCodes.xlsx
+++ b/InputFiles/CRDC/BackupCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Downloads\Commons_Automation\InputFiles\CRDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/ccdi-03-01-2024/Commons_Automation/InputFiles/CRDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB5EDC1-62F7-4C9A-8622-A7B94F0840C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BDBAB1-FF75-214D-96A9-8D02621D795B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sec-codes" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>sec-backup-codes</t>
-  </si>
-  <si>
-    <t>HKDJB5BA6J6M</t>
-  </si>
-  <si>
-    <t>04F5PQ59MWV6</t>
-  </si>
-  <si>
-    <t>95SY88G93C56</t>
   </si>
   <si>
     <t>C9DEXVFAR31A</t>
@@ -382,62 +373,47 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>